<commit_message>
add connections for most recent versions
</commit_message>
<xml_diff>
--- a/CANMFA_Anschluss.xlsx
+++ b/CANMFA_Anschluss.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="87">
   <si>
     <t>T20</t>
   </si>
@@ -260,6 +262,21 @@
   </si>
   <si>
     <t>58b</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t>V0.2</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>NoCAN</t>
+  </si>
+  <si>
+    <t>V1.1</t>
   </si>
 </sst>
 </file>
@@ -401,6 +418,104 @@
         <a:xfrm>
           <a:off x="609600" y="4206240"/>
           <a:ext cx="533446" cy="1135478"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533446</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="4419600"/>
+          <a:ext cx="533446" cy="1181198"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533446</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="4572000"/>
+          <a:ext cx="533446" cy="1181198"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -699,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,6 +826,11 @@
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
@@ -1309,4 +1429,1252 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="3">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="4">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="3">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="4">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor things - add connection plans for v1.1 and v1.2
</commit_message>
<xml_diff>
--- a/CANMFA_Anschluss.xlsx
+++ b/CANMFA_Anschluss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add schematics for V1.1 and V1.2
</commit_message>
<xml_diff>
--- a/CANMFA_Anschluss.xlsx
+++ b/CANMFA_Anschluss.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="104">
   <si>
     <t>T20</t>
   </si>
@@ -277,6 +277,57 @@
   </si>
   <si>
     <t>V1.1</t>
+  </si>
+  <si>
+    <t>KL30</t>
+  </si>
+  <si>
+    <t>KL15</t>
+  </si>
+  <si>
+    <t>KL58b</t>
+  </si>
+  <si>
+    <t>K-Line</t>
+  </si>
+  <si>
+    <t>MFA_Hebel</t>
+  </si>
+  <si>
+    <t>aux_temp</t>
+  </si>
+  <si>
+    <t>oiltemp</t>
+  </si>
+  <si>
+    <t>Gearbox_temp</t>
+  </si>
+  <si>
+    <t>Manifold</t>
+  </si>
+  <si>
+    <t>Starterbat</t>
+  </si>
+  <si>
+    <t>Zweitbat</t>
+  </si>
+  <si>
+    <t>D+/nc</t>
+  </si>
+  <si>
+    <t>Reverse</t>
+  </si>
+  <si>
+    <t>OilTemp</t>
+  </si>
+  <si>
+    <t>StartstopBat</t>
+  </si>
+  <si>
+    <t>GetrTemp</t>
+  </si>
+  <si>
+    <t>Innetemp</t>
   </si>
 </sst>
 </file>
@@ -528,9 +579,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -568,9 +619,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -605,7 +656,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -640,7 +691,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -814,24 +865,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -866,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -895,7 +946,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -918,7 +969,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -941,7 +992,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -964,7 +1015,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -987,7 +1038,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1010,7 +1061,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1033,7 +1084,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1056,7 +1107,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1085,7 +1136,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1114,7 +1165,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1143,7 +1194,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1172,7 +1223,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1201,7 +1252,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1230,7 +1281,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1259,7 +1310,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1288,7 +1339,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1317,7 +1368,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1346,7 +1397,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1375,7 +1426,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1404,7 +1455,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1422,6 +1473,214 @@
       </c>
       <c r="F23" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>18</v>
+      </c>
+      <c r="B49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>19</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>20</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>23</v>
+      </c>
+      <c r="B54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>24</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>25</v>
+      </c>
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1433,19 +1692,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -1456,7 +1715,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1491,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1520,7 +1779,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1543,7 +1802,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1566,7 +1825,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1589,7 +1848,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1612,7 +1871,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1635,7 +1894,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1658,7 +1917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1681,7 +1940,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1710,7 +1969,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1739,7 +1998,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1768,7 +2027,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1797,7 +2056,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1826,7 +2085,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1855,7 +2114,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1884,7 +2143,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1913,7 +2172,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1942,7 +2201,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1971,7 +2230,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2000,7 +2259,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2029,7 +2288,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -2047,6 +2306,214 @@
       </c>
       <c r="F23" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>11</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>15</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>23</v>
+      </c>
+      <c r="B55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>24</v>
+      </c>
+      <c r="B56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>25</v>
+      </c>
+      <c r="B57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2057,19 +2524,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C34" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -2080,7 +2548,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2115,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2144,7 +2612,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2167,7 +2635,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2190,7 +2658,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2213,7 +2681,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2236,7 +2704,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2259,7 +2727,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2282,7 +2750,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2305,7 +2773,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2334,7 +2802,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2363,7 +2831,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2392,7 +2860,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2421,7 +2889,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2450,7 +2918,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2479,7 +2947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2508,7 +2976,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2537,7 +3005,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2566,7 +3034,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2595,7 +3063,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2624,7 +3092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2653,7 +3121,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -2671,6 +3139,214 @@
       </c>
       <c r="F23" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>18</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>19</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>20</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>23</v>
+      </c>
+      <c r="B54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>24</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>25</v>
+      </c>
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make small text display more self-adjusting due to measured adc values
</commit_message>
<xml_diff>
--- a/CANMFA_Anschluss.xlsx
+++ b/CANMFA_Anschluss.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="106">
   <si>
     <t>T20</t>
   </si>
@@ -328,6 +328,12 @@
   </si>
   <si>
     <t>Innetemp</t>
+  </si>
+  <si>
+    <t>MFA</t>
+  </si>
+  <si>
+    <t>BB</t>
   </si>
 </sst>
 </file>
@@ -579,9 +585,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -619,9 +625,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -656,7 +662,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -691,7 +697,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -867,22 +873,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -917,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -946,7 +952,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -969,7 +975,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -992,7 +998,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1015,7 +1021,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1165,7 +1171,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1339,7 +1345,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1426,7 +1432,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1475,7 +1481,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1491,7 +1497,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1499,7 +1505,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1507,7 +1513,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5</v>
       </c>
@@ -1515,7 +1521,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>6</v>
       </c>
@@ -1523,7 +1529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>7</v>
       </c>
@@ -1531,7 +1537,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -1539,7 +1545,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>9</v>
       </c>
@@ -1547,7 +1553,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10</v>
       </c>
@@ -1555,7 +1561,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>11</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>12</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>13</v>
       </c>
@@ -1579,7 +1585,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>14</v>
       </c>
@@ -1587,7 +1593,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>15</v>
       </c>
@@ -1595,7 +1601,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>16</v>
       </c>
@@ -1603,7 +1609,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>17</v>
       </c>
@@ -1611,7 +1617,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>18</v>
       </c>
@@ -1619,7 +1625,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>19</v>
       </c>
@@ -1627,7 +1633,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>20</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>21</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>22</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>23</v>
       </c>
@@ -1659,7 +1665,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>24</v>
       </c>
@@ -1667,7 +1673,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>25</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>26</v>
       </c>
@@ -1694,17 +1700,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:B58"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -1715,7 +1722,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1750,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1779,7 +1786,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1802,7 +1809,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1825,7 +1832,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1848,7 +1855,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1871,7 +1878,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1894,7 +1901,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1917,7 +1924,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1940,7 +1947,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1969,7 +1976,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1998,7 +2005,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2027,7 +2034,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2056,7 +2063,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2085,7 +2092,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2114,7 +2121,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2143,7 +2150,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2172,7 +2179,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2201,7 +2208,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2259,7 +2266,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2288,7 +2295,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -2308,212 +2315,298 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
       <c r="B35" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
       <c r="B36" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>5</v>
       </c>
       <c r="B37" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>6</v>
       </c>
       <c r="B38" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>7</v>
       </c>
       <c r="B39" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
       <c r="B40" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>9</v>
       </c>
       <c r="B41" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10</v>
       </c>
       <c r="B42" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>11</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>12</v>
       </c>
       <c r="B44" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>13</v>
       </c>
       <c r="B45" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>14</v>
       </c>
       <c r="B46" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>15</v>
       </c>
       <c r="B47" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>16</v>
       </c>
       <c r="B48" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>17</v>
       </c>
       <c r="B49" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>18</v>
       </c>
       <c r="B50" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>19</v>
       </c>
       <c r="B51" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>20</v>
       </c>
       <c r="B52" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>21</v>
       </c>
       <c r="B53" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>22</v>
       </c>
       <c r="B54" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>23</v>
       </c>
       <c r="B55" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>24</v>
       </c>
       <c r="B56" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>25</v>
       </c>
       <c r="B57" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>26</v>
       </c>
       <c r="B58" t="s">
         <v>25</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2530,14 +2623,14 @@
       <selection activeCell="C34" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -2548,7 +2641,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2583,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2612,7 +2705,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2635,7 +2728,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2658,7 +2751,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2681,7 +2774,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2704,7 +2797,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2727,7 +2820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2750,7 +2843,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2773,7 +2866,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2802,7 +2895,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2831,7 +2924,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2860,7 +2953,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2889,7 +2982,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2918,7 +3011,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2947,7 +3040,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2976,7 +3069,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3005,7 +3098,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3034,7 +3127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3063,7 +3156,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3092,7 +3185,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3121,7 +3214,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -3141,7 +3234,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -3149,7 +3242,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -3157,7 +3250,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -3165,7 +3258,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3173,7 +3266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5</v>
       </c>
@@ -3181,7 +3274,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>6</v>
       </c>
@@ -3189,7 +3282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>7</v>
       </c>
@@ -3197,7 +3290,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -3205,7 +3298,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>9</v>
       </c>
@@ -3213,7 +3306,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10</v>
       </c>
@@ -3221,7 +3314,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>11</v>
       </c>
@@ -3229,7 +3322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>12</v>
       </c>
@@ -3237,7 +3330,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>13</v>
       </c>
@@ -3245,7 +3338,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>14</v>
       </c>
@@ -3253,7 +3346,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>15</v>
       </c>
@@ -3261,7 +3354,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>16</v>
       </c>
@@ -3269,7 +3362,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>17</v>
       </c>
@@ -3277,7 +3370,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>18</v>
       </c>
@@ -3285,7 +3378,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>19</v>
       </c>
@@ -3293,7 +3386,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>20</v>
       </c>
@@ -3301,7 +3394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>21</v>
       </c>
@@ -3309,7 +3402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>22</v>
       </c>
@@ -3317,7 +3410,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>23</v>
       </c>
@@ -3325,7 +3418,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>24</v>
       </c>
@@ -3333,7 +3426,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>25</v>
       </c>
@@ -3341,7 +3434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Fix Settings through GUI
</commit_message>
<xml_diff>
--- a/CANMFA_Anschluss.xlsx
+++ b/CANMFA_Anschluss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1501,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1752,7 +1752,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
         <v>50</v>
@@ -1766,7 +1766,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
         <v>50</v>
@@ -1907,7 +1907,7 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="C39">
         <v>20</v>
@@ -1918,7 +1918,7 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="C40">
         <v>19</v>
@@ -1929,7 +1929,7 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="C41">
         <v>18</v>
@@ -1940,7 +1940,7 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="C42">
         <v>17</v>

</xml_diff>

<commit_message>
add cal values for all voltages and finalize connection diagram for v1.2 - fix menu settings for new values
</commit_message>
<xml_diff>
--- a/CANMFA_Anschluss.xlsx
+++ b/CANMFA_Anschluss.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="v0.2" sheetId="1" r:id="rId1"/>
+    <sheet name="v1.0" sheetId="2" r:id="rId2"/>
+    <sheet name="v1.2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="154">
   <si>
     <t>T20</t>
   </si>
@@ -261,9 +261,6 @@
     <t>CAN</t>
   </si>
   <si>
-    <t>V1.1</t>
-  </si>
-  <si>
     <t>KL30</t>
   </si>
   <si>
@@ -460,6 +457,27 @@
   </si>
   <si>
     <t>STASTO_ADC7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltage </t>
+  </si>
+  <si>
+    <t>ist</t>
+  </si>
+  <si>
+    <t>soll</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>T3b/2</t>
+  </si>
+  <si>
+    <t>T3b/1</t>
   </si>
 </sst>
 </file>
@@ -544,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -552,23 +570,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1022,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1138,7 @@
       <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F3" t="s">
@@ -1212,7 +1283,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
         <v>73</v>
@@ -1241,7 +1312,7 @@
       <c r="D12" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>65</v>
       </c>
       <c r="F12" t="s">
@@ -1265,7 +1336,7 @@
       <c r="D13" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>56</v>
       </c>
       <c r="F13" t="s">
@@ -1289,7 +1360,7 @@
       <c r="D14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>57</v>
       </c>
       <c r="F14" t="s">
@@ -1313,7 +1384,7 @@
       <c r="D15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>58</v>
       </c>
       <c r="F15" t="s">
@@ -1337,7 +1408,7 @@
       <c r="D16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>62</v>
       </c>
       <c r="F16" t="s">
@@ -1361,7 +1432,7 @@
       <c r="D17" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>63</v>
       </c>
       <c r="F17" t="s">
@@ -1481,7 +1552,7 @@
       <c r="D22" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>64</v>
       </c>
       <c r="F22" t="s">
@@ -1514,7 +1585,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E31" t="s">
         <v>0</v>
@@ -1525,10 +1596,10 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1536,10 +1607,10 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1547,10 +1618,10 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1578,7 +1649,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D36">
         <v>4</v>
@@ -1618,7 +1689,7 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -1638,7 +1709,7 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D39">
         <v>5</v>
@@ -1658,7 +1729,7 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D40">
         <v>7</v>
@@ -1678,7 +1749,7 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D41">
         <v>9</v>
@@ -1718,10 +1789,10 @@
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1733,7 +1804,7 @@
         <v>9</v>
       </c>
       <c r="H43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1741,10 +1812,10 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -1756,7 +1827,7 @@
         <v>10</v>
       </c>
       <c r="H44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1764,10 +1835,10 @@
         <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D45">
         <v>19</v>
@@ -1779,7 +1850,7 @@
         <v>11</v>
       </c>
       <c r="H45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1790,7 +1861,7 @@
         <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D46">
         <v>20</v>
@@ -1802,7 +1873,7 @@
         <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1810,10 +1881,10 @@
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D47">
         <v>11</v>
@@ -1825,7 +1896,7 @@
         <v>13</v>
       </c>
       <c r="H47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1833,10 +1904,10 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D48">
         <v>13</v>
@@ -1848,7 +1919,7 @@
         <v>14</v>
       </c>
       <c r="H48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1856,10 +1927,10 @@
         <v>18</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D49">
         <v>15</v>
@@ -1871,7 +1942,7 @@
         <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1882,7 +1953,7 @@
         <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D50">
         <v>17</v>
@@ -1894,7 +1965,7 @@
         <v>16</v>
       </c>
       <c r="H50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1908,7 +1979,7 @@
         <v>17</v>
       </c>
       <c r="H51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1928,7 +1999,7 @@
         <v>18</v>
       </c>
       <c r="H52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1948,7 +2019,7 @@
         <v>19</v>
       </c>
       <c r="H53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1962,7 +2033,7 @@
         <v>20</v>
       </c>
       <c r="H54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2022,7 +2093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -2070,13 +2141,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="2" t="str">
-        <f>Tabelle1!I3</f>
+        <f>'v0.2'!I3</f>
         <v>Solar</v>
       </c>
       <c r="G3" s="2" t="str">
@@ -2098,7 +2169,7 @@
         <v>42</v>
       </c>
       <c r="F4" t="str">
-        <f>Tabelle1!I4</f>
+        <f>'v0.2'!I4</f>
         <v>SDA</v>
       </c>
       <c r="G4" t="str">
@@ -2120,7 +2191,7 @@
         <v>42</v>
       </c>
       <c r="F5" t="str">
-        <f>Tabelle1!I5</f>
+        <f>'v0.2'!I5</f>
         <v>SCL</v>
       </c>
       <c r="G5" t="str">
@@ -2142,7 +2213,7 @@
         <v>43</v>
       </c>
       <c r="F6" t="str">
-        <f>Tabelle1!I6</f>
+        <f>'v0.2'!I6</f>
         <v>GND</v>
       </c>
       <c r="G6" t="str">
@@ -2164,7 +2235,7 @@
         <v>43</v>
       </c>
       <c r="F7" t="str">
-        <f>Tabelle1!I7</f>
+        <f>'v0.2'!I7</f>
         <v>GND</v>
       </c>
       <c r="G7" t="str">
@@ -2186,7 +2257,7 @@
         <v>44</v>
       </c>
       <c r="F8" t="str">
-        <f>Tabelle1!I8</f>
+        <f>'v0.2'!I8</f>
         <v>CANH</v>
       </c>
       <c r="G8" t="str">
@@ -2208,7 +2279,7 @@
         <v>44</v>
       </c>
       <c r="F9" t="str">
-        <f>Tabelle1!I9</f>
+        <f>'v0.2'!I9</f>
         <v>CANL</v>
       </c>
       <c r="G9" t="str">
@@ -2230,7 +2301,7 @@
         <v>45</v>
       </c>
       <c r="F10" t="str">
-        <f>Tabelle1!I10</f>
+        <f>'v0.2'!I10</f>
         <v>TKML</v>
       </c>
       <c r="G10" t="str">
@@ -2246,13 +2317,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
         <v>73</v>
       </c>
       <c r="F11" s="4" t="str">
-        <f>Tabelle1!I11</f>
+        <f>'v0.2'!I11</f>
         <v>REV</v>
       </c>
       <c r="G11" s="4" t="str">
@@ -2268,16 +2339,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" t="s">
         <v>108</v>
       </c>
-      <c r="D12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="6" t="str">
-        <f>Tabelle1!I12</f>
+      <c r="F12" s="5" t="str">
+        <f>'v0.2'!I12</f>
         <v>GT_ADC6</v>
       </c>
-      <c r="G12" s="6" t="str">
+      <c r="G12" s="5" t="str">
         <f t="shared" si="0"/>
         <v>OT_ADC1</v>
       </c>
@@ -2293,10 +2364,10 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" s="2" t="str">
-        <f>Tabelle1!I13</f>
+        <f>'v0.2'!I13</f>
         <v>STST_ADC5</v>
       </c>
       <c r="G13" s="2" t="str">
@@ -2312,13 +2383,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F14" s="2" t="str">
-        <f>Tabelle1!I14</f>
+        <f>'v0.2'!I14</f>
         <v>AT_ADC0</v>
       </c>
       <c r="G14" s="2" t="str">
@@ -2340,7 +2411,7 @@
         <v>41</v>
       </c>
       <c r="F15" s="2" t="str">
-        <f>Tabelle1!I15</f>
+        <f>'v0.2'!I15</f>
         <v>OT_ADC1</v>
       </c>
       <c r="G15" s="2" t="str">
@@ -2359,10 +2430,10 @@
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F16" s="3" t="str">
-        <f>Tabelle1!I16</f>
+        <f>'v0.2'!I16</f>
         <v>SB_ADC2</v>
       </c>
       <c r="G16" s="3" t="str">
@@ -2381,10 +2452,10 @@
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F17" s="3" t="str">
-        <f>Tabelle1!I17</f>
+        <f>'v0.2'!I17</f>
         <v>ZB_ADC3</v>
       </c>
       <c r="G17" s="3" t="str">
@@ -2406,7 +2477,7 @@
         <v>50</v>
       </c>
       <c r="F18" t="str">
-        <f>Tabelle1!I18</f>
+        <f>'v0.2'!I18</f>
         <v>MFA_HEBEL</v>
       </c>
       <c r="G18" t="str">
@@ -2428,7 +2499,7 @@
         <v>50</v>
       </c>
       <c r="F19" t="str">
-        <f>Tabelle1!I19</f>
+        <f>'v0.2'!I19</f>
         <v>MFA_HEBEL</v>
       </c>
       <c r="G19" t="str">
@@ -2450,7 +2521,7 @@
         <v>50</v>
       </c>
       <c r="F20" t="str">
-        <f>Tabelle1!I20</f>
+        <f>'v0.2'!I20</f>
         <v>MFA_HEBEL</v>
       </c>
       <c r="G20" t="str">
@@ -2472,7 +2543,7 @@
         <v>50</v>
       </c>
       <c r="F21" t="str">
-        <f>Tabelle1!I21</f>
+        <f>'v0.2'!I21</f>
         <v>MFA_HEBEL</v>
       </c>
       <c r="G21" t="str">
@@ -2491,10 +2562,10 @@
         <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F22" s="3" t="str">
-        <f>Tabelle1!I22</f>
+        <f>'v0.2'!I22</f>
         <v>IT-ADC7</v>
       </c>
       <c r="G22" s="3" t="str">
@@ -2518,13 +2589,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s">
         <v>99</v>
       </c>
-      <c r="C32" t="s">
-        <v>100</v>
-      </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E32" t="s">
         <v>0</v>
@@ -2535,13 +2606,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33">
         <v>26</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2549,13 +2620,13 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34">
         <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2563,13 +2634,13 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35">
         <v>24</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2592,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2600,7 +2671,7 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37">
         <v>22</v>
@@ -2761,7 +2832,7 @@
         <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C44">
         <v>15</v>
@@ -2776,7 +2847,7 @@
         <v>9</v>
       </c>
       <c r="H44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2784,7 +2855,7 @@
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45">
         <v>14</v>
@@ -2799,7 +2870,7 @@
         <v>10</v>
       </c>
       <c r="H45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2807,7 +2878,7 @@
         <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C46">
         <v>13</v>
@@ -2822,7 +2893,7 @@
         <v>11</v>
       </c>
       <c r="H46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2830,7 +2901,7 @@
         <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47">
         <v>12</v>
@@ -2845,7 +2916,7 @@
         <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2853,7 +2924,7 @@
         <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C48">
         <v>11</v>
@@ -2868,7 +2939,7 @@
         <v>13</v>
       </c>
       <c r="H48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2876,7 +2947,7 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49">
         <v>10</v>
@@ -2891,7 +2962,7 @@
         <v>14</v>
       </c>
       <c r="H49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2914,7 +2985,7 @@
         <v>15</v>
       </c>
       <c r="H50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2922,7 +2993,7 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C51">
         <v>8</v>
@@ -2937,7 +3008,7 @@
         <v>16</v>
       </c>
       <c r="H51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2954,7 +3025,7 @@
         <v>17</v>
       </c>
       <c r="H52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2977,7 +3048,7 @@
         <v>18</v>
       </c>
       <c r="H53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3000,7 +3071,7 @@
         <v>19</v>
       </c>
       <c r="H54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3017,7 +3088,7 @@
         <v>20</v>
       </c>
       <c r="H55" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3083,88 +3154,110 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>81</v>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="I1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H1" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="G2" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="11"/>
+      <c r="O2" t="s">
+        <v>147</v>
+      </c>
+      <c r="P2" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="F3" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="2" t="str">
-        <f>Tabelle1!I3</f>
-        <v>Solar</v>
-      </c>
-      <c r="H3" s="2" t="str">
+      <c r="G3" t="str">
         <f>H35</f>
         <v>MAN_ADC3</v>
       </c>
-      <c r="I3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="H3" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" t="s">
+        <v>150</v>
+      </c>
+      <c r="P3">
+        <v>17.78</v>
+      </c>
+      <c r="Q3">
+        <v>12.3</v>
+      </c>
+      <c r="S3">
+        <f>P3/128*171</f>
+        <v>23.752968750000001</v>
+      </c>
+      <c r="T3">
+        <f>Q3/128*185</f>
+        <v>17.77734375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -3177,19 +3270,29 @@
         <v>42</v>
       </c>
       <c r="G4" t="str">
-        <f>Tabelle1!I4</f>
+        <f t="shared" ref="G4:G22" si="0">H36</f>
         <v>SDA</v>
       </c>
-      <c r="H4" t="str">
-        <f t="shared" ref="H4:H22" si="0">H36</f>
-        <v>SDA</v>
-      </c>
-      <c r="I4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="H4" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="P4">
+        <v>17.78</v>
+      </c>
+      <c r="Q4">
+        <v>12.3</v>
+      </c>
+      <c r="S4">
+        <f>P4/128*171</f>
+        <v>23.752968750000001</v>
+      </c>
+      <c r="T4">
+        <f>Q4/128*185</f>
+        <v>17.77734375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -3202,19 +3305,25 @@
         <v>42</v>
       </c>
       <c r="G5" t="str">
-        <f>Tabelle1!I5</f>
+        <f t="shared" si="0"/>
         <v>SCL</v>
       </c>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>SCL</v>
-      </c>
-      <c r="I5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="H5" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="P5">
+        <v>13.3</v>
+      </c>
+      <c r="Q5">
+        <v>12.23</v>
+      </c>
+      <c r="T5">
+        <f>P6/P5*Q5</f>
+        <v>117.70225563909774</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -3227,16 +3336,23 @@
         <v>43</v>
       </c>
       <c r="G6" t="str">
-        <f>Tabelle1!I6</f>
+        <f t="shared" si="0"/>
         <v>GND</v>
       </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>GND</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="H6" s="14"/>
+      <c r="P6">
+        <v>128</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>151</v>
+      </c>
+      <c r="T6" t="e">
+        <f t="shared" ref="T6" si="1">Q6/128*185</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -3249,16 +3365,13 @@
         <v>43</v>
       </c>
       <c r="G7" t="str">
-        <f>Tabelle1!I7</f>
+        <f t="shared" si="0"/>
         <v>GND</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>GND</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -3271,16 +3384,13 @@
         <v>44</v>
       </c>
       <c r="G8" t="str">
-        <f>Tabelle1!I8</f>
+        <f t="shared" si="0"/>
         <v>CANH</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>CANH</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -3293,16 +3403,13 @@
         <v>44</v>
       </c>
       <c r="G9" t="str">
-        <f>Tabelle1!I9</f>
+        <f t="shared" si="0"/>
         <v>CANL</v>
       </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>CANL</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -3315,23 +3422,20 @@
         <v>45</v>
       </c>
       <c r="G10" t="str">
-        <f>Tabelle1!I10</f>
+        <f t="shared" si="0"/>
         <v>TKML</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>TKML</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
         <v>73</v>
@@ -3342,89 +3446,78 @@
       <c r="F11" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="4" t="str">
-        <f>Tabelle1!I11</f>
-        <v>REV</v>
-      </c>
-      <c r="H11" s="4" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>KLINE</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" t="s">
         <v>108</v>
       </c>
-      <c r="D12" t="s">
-        <v>109</v>
-      </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="3" t="str">
-        <f>Tabelle1!I12</f>
-        <v>GT_ADC6</v>
-      </c>
-      <c r="H12" s="3" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="0"/>
         <v>OT_ADC1</v>
       </c>
+      <c r="H12" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="I12" t="s">
-        <v>77</v>
-      </c>
-      <c r="J12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>152</v>
       </c>
       <c r="F13" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="2" t="str">
-        <f>Tabelle1!I13</f>
-        <v>STST_ADC5</v>
-      </c>
-      <c r="H13" s="2" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>GT_ADC2</v>
       </c>
+      <c r="H13" s="14" t="s">
+        <v>71</v>
+      </c>
       <c r="I13" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -3433,32 +3526,28 @@
         <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="5" t="str">
-        <f>Tabelle1!I14</f>
-        <v>AT_ADC0</v>
-      </c>
-      <c r="H14" s="5" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>STASTO_ADC7</v>
       </c>
+      <c r="H14" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="I14" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -3467,90 +3556,79 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="2" t="str">
-        <f>Tabelle1!I15</f>
-        <v>OT_ADC1</v>
-      </c>
-      <c r="H15" s="2" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>S_ADC6</v>
       </c>
+      <c r="H15" s="14" t="s">
+        <v>110</v>
+      </c>
       <c r="I15" t="s">
-        <v>111</v>
-      </c>
-      <c r="J15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="3" t="str">
-        <f>Tabelle1!I16</f>
-        <v>SB_ADC2</v>
-      </c>
-      <c r="H16" s="3" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>ZB_ADC5</v>
       </c>
+      <c r="H16" s="14" t="s">
+        <v>109</v>
+      </c>
       <c r="I16" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="3" t="str">
-        <f>Tabelle1!I17</f>
-        <v>ZB_ADC3</v>
-      </c>
-      <c r="H17" s="3" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>SB_ADC4</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -3569,16 +3647,13 @@
         <v>61</v>
       </c>
       <c r="G18" t="str">
-        <f>Tabelle1!I18</f>
+        <f t="shared" si="0"/>
         <v>MFA_HEBEL</v>
       </c>
-      <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v>MFA_HEBEL</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -3597,16 +3672,13 @@
         <v>61</v>
       </c>
       <c r="G19" t="str">
-        <f>Tabelle1!I19</f>
+        <f t="shared" si="0"/>
         <v>MFA_HEBEL</v>
       </c>
-      <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v>MFA_HEBEL</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -3625,16 +3697,13 @@
         <v>61</v>
       </c>
       <c r="G20" t="str">
-        <f>Tabelle1!I20</f>
+        <f t="shared" si="0"/>
         <v>MFA_HEBEL</v>
       </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v>MFA_HEBEL</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -3653,46 +3722,39 @@
         <v>61</v>
       </c>
       <c r="G21" t="str">
-        <f>Tabelle1!I21</f>
+        <f t="shared" si="0"/>
         <v>MFA_HEBEL</v>
       </c>
-      <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v>MFA_HEBEL</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E22" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="3" t="str">
-        <f>Tabelle1!I22</f>
-        <v>IT-ADC7</v>
-      </c>
-      <c r="H22" s="3" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v>AT_ADC0</v>
       </c>
-      <c r="I22" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -3712,23 +3774,23 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E31" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3736,10 +3798,10 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3747,10 +3809,10 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3770,7 +3832,7 @@
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3778,7 +3840,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36">
         <v>4</v>
@@ -3818,7 +3880,7 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -3838,7 +3900,7 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D39">
         <v>5</v>
@@ -3858,7 +3920,7 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D40">
         <v>7</v>
@@ -3878,7 +3940,7 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D41">
         <v>9</v>
@@ -3918,10 +3980,10 @@
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3933,7 +3995,7 @@
         <v>9</v>
       </c>
       <c r="H43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3941,10 +4003,10 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -3956,7 +4018,7 @@
         <v>10</v>
       </c>
       <c r="H44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3964,10 +4026,10 @@
         <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D45">
         <v>19</v>
@@ -3979,7 +4041,7 @@
         <v>11</v>
       </c>
       <c r="H45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3987,10 +4049,10 @@
         <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D46">
         <v>20</v>
@@ -4002,7 +4064,7 @@
         <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -4010,10 +4072,10 @@
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D47">
         <v>11</v>
@@ -4025,7 +4087,7 @@
         <v>13</v>
       </c>
       <c r="H47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -4033,10 +4095,10 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D48">
         <v>13</v>
@@ -4048,7 +4110,7 @@
         <v>14</v>
       </c>
       <c r="H48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -4059,7 +4121,7 @@
         <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D49">
         <v>15</v>
@@ -4071,7 +4133,7 @@
         <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -4079,10 +4141,10 @@
         <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C50" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D50">
         <v>17</v>
@@ -4094,7 +4156,7 @@
         <v>16</v>
       </c>
       <c r="H50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4108,7 +4170,7 @@
         <v>17</v>
       </c>
       <c r="H51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -4128,7 +4190,7 @@
         <v>18</v>
       </c>
       <c r="H52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4148,7 +4210,7 @@
         <v>19</v>
       </c>
       <c r="H53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -4162,7 +4224,7 @@
         <v>20</v>
       </c>
       <c r="H54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
try to fix stuff
</commit_message>
<xml_diff>
--- a/CANMFA_Anschluss.xlsx
+++ b/CANMFA_Anschluss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="v0.2" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="v1.2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1093,7 +1094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -3156,8 +3157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3347,7 +3348,7 @@
         <v>151</v>
       </c>
       <c r="T6" t="e">
-        <f t="shared" ref="T6" si="1">Q6/128*185</f>
+        <f>Q6/128*185</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>